<commit_message>
Add fastq + analysis
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.32.taxprofiler.xlsx
+++ b/tests/fixtures/orderforms/1508.32.taxprofiler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isakohlsson/dev/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A544D91D-3CBE-3947-AE08-F9852F4B0B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714D8A18-11FF-7446-BF16-69545AEF355D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30440" windowHeight="17500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30440" windowHeight="16260" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -5529,7 +5529,7 @@
   </sheetPr>
   <dimension ref="A1:AMO395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D15" sqref="D15:D34"/>
     </sheetView>
   </sheetViews>
@@ -14296,7 +14296,7 @@
         <v>617</v>
       </c>
       <c r="D16" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E16" s="68" t="s">
         <v>730</v>
@@ -16418,7 +16418,7 @@
         <v>617</v>
       </c>
       <c r="D18" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E18" s="68" t="s">
         <v>734</v>
@@ -18538,7 +18538,7 @@
         <v>617</v>
       </c>
       <c r="D20" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E20" s="68" t="s">
         <v>738</v>
@@ -20658,7 +20658,7 @@
         <v>617</v>
       </c>
       <c r="D22" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E22" s="68" t="s">
         <v>742</v>
@@ -22778,7 +22778,7 @@
         <v>617</v>
       </c>
       <c r="D24" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E24" s="68" t="s">
         <v>746</v>
@@ -24898,7 +24898,7 @@
         <v>617</v>
       </c>
       <c r="D26" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E26" s="68" t="s">
         <v>750</v>
@@ -26028,7 +26028,7 @@
         <v>617</v>
       </c>
       <c r="D28" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E28" s="68" t="s">
         <v>754</v>
@@ -28148,7 +28148,7 @@
         <v>617</v>
       </c>
       <c r="D30" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E30" s="68" t="s">
         <v>758</v>
@@ -30268,7 +30268,7 @@
         <v>617</v>
       </c>
       <c r="D32" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E32" s="68" t="s">
         <v>762</v>
@@ -32388,7 +32388,7 @@
         <v>617</v>
       </c>
       <c r="D34" s="68" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="E34" s="68" t="s">
         <v>766</v>

</xml_diff>